<commit_message>
document add and login only email
</commit_message>
<xml_diff>
--- a/Document_Api/API-V-0.4.xlsx
+++ b/Document_Api/API-V-0.4.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="138">
   <si>
     <t>Base URL:</t>
   </si>
@@ -403,9 +403,6 @@
     <t>logout and remove access token</t>
   </si>
   <si>
-    <t>username,password</t>
-  </si>
-  <si>
     <t>access_token</t>
   </si>
   <si>
@@ -418,25 +415,19 @@
     <t>http://www.freewebs.co.in/mobiapp/apis/list?model=Product</t>
   </si>
   <si>
-    <t>http://www.freewebs.co.in/mobiapp/apis/list?model=Users</t>
-  </si>
-  <si>
-    <t>Get list off all users</t>
-  </si>
-  <si>
     <t>Get list off all product</t>
   </si>
   <si>
     <t>Get list off all vendor (same as getAllVendorList)</t>
   </si>
   <si>
-    <t>Post request model=Users required</t>
-  </si>
-  <si>
     <t>Post request model=Product required</t>
   </si>
   <si>
     <t>Post request model=Vendor required</t>
+  </si>
+  <si>
+    <t>email,password</t>
   </si>
 </sst>
 </file>
@@ -917,7 +908,7 @@
   <dimension ref="A1:P774"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2188,7 +2179,7 @@
         <v>127</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -2218,7 +2209,7 @@
         <v>128</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -2251,7 +2242,7 @@
     </row>
     <row r="50" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="7"/>
@@ -2287,24 +2278,12 @@
       <c r="P51" s="3"/>
     </row>
     <row r="52" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F52" s="19" t="s">
-        <v>138</v>
-      </c>
+      <c r="A52" s="3"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="19"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
@@ -2327,13 +2306,13 @@
         <v>6</v>
       </c>
       <c r="D53" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="E53" s="6" t="s">
-        <v>136</v>
-      </c>
       <c r="F53" s="19" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
@@ -2357,13 +2336,13 @@
         <v>6</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -15352,9 +15331,8 @@
     <hyperlink ref="D48" r:id="rId12"/>
     <hyperlink ref="D54" r:id="rId13"/>
     <hyperlink ref="D53" r:id="rId14"/>
-    <hyperlink ref="D52" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>